<commit_message>
3rd commit and step 3 for katalon certification
</commit_message>
<xml_diff>
--- a/Drivers/Data file1.xlsx
+++ b/Drivers/Data file1.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RavishankarN\Katalon Studio\Certification project\Drivers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D9CAD6-885D-4162-8B27-4B81D9FD7C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619B2D30-D05E-4B78-93A0-38CD5E81204D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{174463BA-0C40-42A6-B5A0-50603AE645F9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{174463BA-0C40-42A6-B5A0-50603AE645F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="64">
   <si>
     <t>Password</t>
   </si>
@@ -104,24 +105,12 @@
     <t>07/21/2024</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>First Name</t>
   </si>
   <si>
-    <t>Last Name</t>
-  </si>
-  <si>
     <t>Message</t>
   </si>
   <si>
-    <t>Name1</t>
-  </si>
-  <si>
-    <t>Test1testing1@yopmail.com</t>
-  </si>
-  <si>
     <t>Test1contact1</t>
   </si>
   <si>
@@ -131,66 +120,36 @@
     <t>Message contact 1</t>
   </si>
   <si>
-    <t>Name2</t>
-  </si>
-  <si>
     <t>Test1contact2</t>
   </si>
   <si>
     <t>Message contact 2</t>
   </si>
   <si>
-    <t>Name3</t>
-  </si>
-  <si>
     <t>Test1contact3</t>
   </si>
   <si>
     <t>Message contact 3</t>
   </si>
   <si>
-    <t>Name4</t>
-  </si>
-  <si>
     <t>Test1contact4</t>
   </si>
   <si>
     <t>Message contact 4</t>
   </si>
   <si>
-    <t>Name5</t>
-  </si>
-  <si>
     <t>Test1contact5</t>
   </si>
   <si>
     <t>Message contact 5</t>
   </si>
   <si>
-    <t>Name6</t>
-  </si>
-  <si>
     <t>Test1contact6</t>
   </si>
   <si>
     <t>Message contact 6</t>
   </si>
   <si>
-    <t>Test2testing1@yopmail.com</t>
-  </si>
-  <si>
-    <t>Test3testing1@yopmail.com</t>
-  </si>
-  <si>
-    <t>Test4testing1@yopmail.com</t>
-  </si>
-  <si>
-    <t>Test5testing1@yopmail.com</t>
-  </si>
-  <si>
-    <t>Test6testing1@yopmail.com</t>
-  </si>
-  <si>
     <t>Fstname2testing1@yopmail.com</t>
   </si>
   <si>
@@ -204,6 +163,75 @@
   </si>
   <si>
     <t>Fstname6testing1@yopmail.com</t>
+  </si>
+  <si>
+    <t>First_Name</t>
+  </si>
+  <si>
+    <t>Last_Name</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>Words</t>
+  </si>
+  <si>
+    <t>Test contact1</t>
+  </si>
+  <si>
+    <t>First1</t>
+  </si>
+  <si>
+    <t>Mid2</t>
+  </si>
+  <si>
+    <t>Last3</t>
+  </si>
+  <si>
+    <t>Test contact2</t>
+  </si>
+  <si>
+    <t>First2</t>
+  </si>
+  <si>
+    <t>Mid3</t>
+  </si>
+  <si>
+    <t>Last4</t>
+  </si>
+  <si>
+    <t>Test contact3</t>
+  </si>
+  <si>
+    <t>First3</t>
+  </si>
+  <si>
+    <t>Mid4</t>
+  </si>
+  <si>
+    <t>Last5</t>
+  </si>
+  <si>
+    <t>Key_word</t>
+  </si>
+  <si>
+    <t>contact_name</t>
+  </si>
+  <si>
+    <t>First_name</t>
+  </si>
+  <si>
+    <t>Mid_name</t>
+  </si>
+  <si>
+    <t>Last_name</t>
   </si>
 </sst>
 </file>
@@ -808,178 +836,245 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E474BE93-65F3-4B21-A5E0-20586D32FD1A}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>21</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B2" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="C2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="D2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
         <v>26</v>
       </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
         <v>27</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
         <v>28</v>
       </c>
-      <c r="F2" t="s">
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
         <v>30</v>
       </c>
-      <c r="B3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
         <v>31</v>
       </c>
-      <c r="E3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
         <v>33</v>
       </c>
-      <c r="B4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
         <v>34</v>
       </c>
-      <c r="E4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{7053622F-387B-442C-BE79-B81BD93F02E9}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{739D64CC-2894-4280-A96F-4448BAFAC83C}"/>
-    <hyperlink ref="B3" r:id="rId3" xr:uid="{4355DD3B-0B99-4FE7-953B-695610CF0E15}"/>
-    <hyperlink ref="B4" r:id="rId4" xr:uid="{7A591E5E-917F-4135-8A23-6D305043D5C8}"/>
-    <hyperlink ref="B5" r:id="rId5" xr:uid="{5AB06460-917A-4AA8-BEF8-DF296C74A472}"/>
-    <hyperlink ref="B6" r:id="rId6" xr:uid="{2F095182-AA11-4A1D-9DE2-1EA45B73DC87}"/>
-    <hyperlink ref="B7" r:id="rId7" xr:uid="{BC02A392-9F54-4490-9E09-EA5E862E3D49}"/>
-    <hyperlink ref="E3" r:id="rId8" xr:uid="{53323E75-AB01-48A7-A5B0-6E03ABB819CE}"/>
-    <hyperlink ref="E4" r:id="rId9" xr:uid="{B4DCB193-1559-4823-B4AD-7AFF05DB97A6}"/>
-    <hyperlink ref="E5" r:id="rId10" xr:uid="{9DF275B5-3EA1-4DBD-84A5-867067E77D6C}"/>
-    <hyperlink ref="E6" r:id="rId11" xr:uid="{3E9E976C-BB35-4FB1-81C8-773566CFA3C4}"/>
-    <hyperlink ref="E7" r:id="rId12" xr:uid="{788DB658-9B20-4833-B157-066B05E009B3}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{739D64CC-2894-4280-A96F-4448BAFAC83C}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{53323E75-AB01-48A7-A5B0-6E03ABB819CE}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{B4DCB193-1559-4823-B4AD-7AFF05DB97A6}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{9DF275B5-3EA1-4DBD-84A5-867067E77D6C}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{3E9E976C-BB35-4FB1-81C8-773566CFA3C4}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{788DB658-9B20-4833-B157-066B05E009B3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F0F541-4FD6-4154-B938-A53EDB6E051A}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>